<commit_message>
Commiting files from jenkins
</commit_message>
<xml_diff>
--- a/src/test/java/com/vajra/TestData/Usernameandpassword.xlsx
+++ b/src/test/java/com/vajra/TestData/Usernameandpassword.xlsx
@@ -399,7 +399,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -424,7 +424,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1">
-        <v>63</v>
+        <v>13</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>

</xml_diff>